<commit_message>
Updated with latest results.
</commit_message>
<xml_diff>
--- a/ml_results.xlsx
+++ b/ml_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timosommer/PhD/projects/others/Manting_Fukui_indices/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timosommer/PhD/projects/others/Fukui-Indices/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D49CCC-9F64-FB4E-A3DE-27089E01FEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A802E1B0-5C87-874D-9E60-F9F514B573D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="500" windowWidth="37080" windowHeight="21100" xr2:uid="{3179A478-D9C7-A448-B85C-D28A6D71322D}"/>
+    <workbookView xWindow="38400" yWindow="1620" windowWidth="28800" windowHeight="17500" xr2:uid="{3179A478-D9C7-A448-B85C-D28A6D71322D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -116,9 +116,6 @@
     <t>dft pca 132</t>
   </si>
   <si>
-    <t>Experiment: hammett</t>
-  </si>
-  <si>
     <t>Hammett</t>
   </si>
   <si>
@@ -149,25 +146,28 @@
     <t>Pred: 0.94, True: 0.06</t>
   </si>
   <si>
-    <t>Experiment: XGBC_seed=1</t>
-  </si>
-  <si>
-    <t>Experiment: XGBC_seed=2</t>
-  </si>
-  <si>
-    <t>Experiment: XGBC_seed=3</t>
-  </si>
-  <si>
-    <t>Experiment: XGBC_seed=4</t>
-  </si>
-  <si>
-    <t>Experiment: XGBC_seed=5</t>
-  </si>
-  <si>
     <t>Experiments: all_models_{features}</t>
   </si>
   <si>
     <t>Wrongly predicted molecules: Probability of wrongly predicted site (Pred) vs probability of actually correct site(s) (True)</t>
+  </si>
+  <si>
+    <t>Experiment: XGBC_seed_1</t>
+  </si>
+  <si>
+    <t>Experiment: XGBC_seed_2</t>
+  </si>
+  <si>
+    <t>Experiment: XGBC_seed_3</t>
+  </si>
+  <si>
+    <t>Experiment: XGBC_seed_4</t>
+  </si>
+  <si>
+    <t>Experiment: XGBC_seed_5</t>
+  </si>
+  <si>
+    <t>Experiment: Hammett</t>
   </si>
 </sst>
 </file>
@@ -253,14 +253,14 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -599,8 +599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B45F95CD-8FA7-A443-A4CD-D9F038324DD6}">
   <dimension ref="A1:S81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -616,18 +616,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F2" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
+      <c r="F2" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
     </row>
     <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -655,18 +655,18 @@
         <v>7</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -697,7 +697,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -730,7 +730,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -763,7 +763,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -796,7 +796,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -829,7 +829,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -842,7 +842,7 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D15" s="3">
         <v>0.88</v>
@@ -851,16 +851,16 @@
         <v>0.94</v>
       </c>
       <c r="F15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -869,12 +869,12 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
@@ -930,7 +930,7 @@
       <c r="E20" s="5">
         <v>0.88</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F20" s="7">
         <v>0.94</v>
       </c>
       <c r="G20" s="4">
@@ -957,10 +957,10 @@
         <v>0.81</v>
       </c>
       <c r="E21" s="4">
-        <v>0.62</v>
+        <v>0.59</v>
       </c>
       <c r="F21" s="4">
-        <v>0.88</v>
+        <v>0.94</v>
       </c>
       <c r="G21" s="4">
         <v>0.81</v>
@@ -977,7 +977,7 @@
         <v>12</v>
       </c>
       <c r="B22" s="4">
-        <v>0.69</v>
+        <v>0.88</v>
       </c>
       <c r="C22" s="5">
         <v>0.84</v>
@@ -986,10 +986,10 @@
         <v>0.94</v>
       </c>
       <c r="E22" s="4">
-        <v>0.41</v>
-      </c>
-      <c r="F22" s="4">
-        <v>0.69</v>
+        <v>0.09</v>
+      </c>
+      <c r="F22" s="5">
+        <v>0.97</v>
       </c>
       <c r="G22" s="5">
         <v>0.91</v>
@@ -998,7 +998,7 @@
         <v>0.91</v>
       </c>
       <c r="I22" s="4">
-        <v>0.56000000000000005</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.2">
@@ -1006,28 +1006,28 @@
         <v>13</v>
       </c>
       <c r="B23" s="4">
-        <v>0.66</v>
+        <v>0.78</v>
       </c>
       <c r="C23" s="4">
         <v>0.81</v>
       </c>
-      <c r="D23" s="5">
-        <v>0.94</v>
+      <c r="D23" s="7">
+        <v>0.91</v>
       </c>
       <c r="E23" s="4">
-        <v>0.06</v>
+        <v>0.03</v>
       </c>
       <c r="F23" s="4">
-        <v>0.62</v>
-      </c>
-      <c r="G23" s="5">
-        <v>0.91</v>
+        <v>0.84</v>
+      </c>
+      <c r="G23" s="7">
+        <v>0.88</v>
       </c>
       <c r="H23" s="4">
         <v>0.88</v>
       </c>
       <c r="I23" s="4">
-        <v>0.03</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.2">
@@ -1035,7 +1035,7 @@
         <v>14</v>
       </c>
       <c r="B24" s="4">
-        <v>0.69</v>
+        <v>0.06</v>
       </c>
       <c r="C24" s="4">
         <v>0.75</v>
@@ -1047,7 +1047,7 @@
         <v>0</v>
       </c>
       <c r="F24" s="4">
-        <v>0.69</v>
+        <v>0.06</v>
       </c>
       <c r="G24" s="4">
         <v>0.81</v>
@@ -1069,7 +1069,7 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
@@ -1113,28 +1113,28 @@
       <c r="A29" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="9">
-        <v>1</v>
-      </c>
-      <c r="C29" s="9">
-        <v>1</v>
-      </c>
-      <c r="D29" s="9">
-        <v>1</v>
-      </c>
-      <c r="E29" s="9">
-        <v>1</v>
-      </c>
-      <c r="F29" s="9">
-        <v>1</v>
-      </c>
-      <c r="G29" s="9">
-        <v>1</v>
-      </c>
-      <c r="H29" s="9">
-        <v>1</v>
-      </c>
-      <c r="I29" s="9">
+      <c r="B29" s="7">
+        <v>1</v>
+      </c>
+      <c r="C29" s="7">
+        <v>1</v>
+      </c>
+      <c r="D29" s="7">
+        <v>1</v>
+      </c>
+      <c r="E29" s="7">
+        <v>1</v>
+      </c>
+      <c r="F29" s="7">
+        <v>1</v>
+      </c>
+      <c r="G29" s="7">
+        <v>1</v>
+      </c>
+      <c r="H29" s="7">
+        <v>1</v>
+      </c>
+      <c r="I29" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1142,28 +1142,28 @@
       <c r="A30" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="9">
-        <v>1</v>
-      </c>
-      <c r="C30" s="9">
-        <v>1</v>
-      </c>
-      <c r="D30" s="9">
-        <v>1</v>
-      </c>
-      <c r="E30" s="9">
-        <v>1</v>
-      </c>
-      <c r="F30" s="9">
-        <v>1</v>
-      </c>
-      <c r="G30" s="9">
-        <v>1</v>
-      </c>
-      <c r="H30" s="9">
-        <v>1</v>
-      </c>
-      <c r="I30" s="9">
+      <c r="B30" s="7">
+        <v>1</v>
+      </c>
+      <c r="C30" s="7">
+        <v>1</v>
+      </c>
+      <c r="D30" s="7">
+        <v>1</v>
+      </c>
+      <c r="E30" s="7">
+        <v>1</v>
+      </c>
+      <c r="F30" s="7">
+        <v>1</v>
+      </c>
+      <c r="G30" s="7">
+        <v>1</v>
+      </c>
+      <c r="H30" s="7">
+        <v>1</v>
+      </c>
+      <c r="I30" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1171,28 +1171,28 @@
       <c r="A31" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="9">
-        <v>0.74</v>
-      </c>
-      <c r="C31" s="9">
+      <c r="B31" s="7">
+        <v>1</v>
+      </c>
+      <c r="C31" s="7">
         <v>0.94</v>
       </c>
-      <c r="D31" s="9">
-        <v>1</v>
-      </c>
-      <c r="E31" s="9">
-        <v>1</v>
-      </c>
-      <c r="F31" s="9">
-        <v>0.76</v>
-      </c>
-      <c r="G31" s="9">
+      <c r="D31" s="7">
+        <v>1</v>
+      </c>
+      <c r="E31" s="7">
+        <v>1</v>
+      </c>
+      <c r="F31" s="7">
+        <v>1</v>
+      </c>
+      <c r="G31" s="7">
         <v>0.97</v>
       </c>
-      <c r="H31" s="9">
-        <v>1</v>
-      </c>
-      <c r="I31" s="9">
+      <c r="H31" s="7">
+        <v>1</v>
+      </c>
+      <c r="I31" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1200,28 +1200,28 @@
       <c r="A32" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="9">
-        <v>0.74</v>
-      </c>
-      <c r="C32" s="9">
-        <v>1</v>
-      </c>
-      <c r="D32" s="9">
-        <v>1</v>
-      </c>
-      <c r="E32" s="9">
-        <v>1</v>
-      </c>
-      <c r="F32" s="9">
-        <v>0.74</v>
-      </c>
-      <c r="G32" s="9">
-        <v>1</v>
-      </c>
-      <c r="H32" s="9">
-        <v>1</v>
-      </c>
-      <c r="I32" s="9">
+      <c r="B32" s="7">
+        <v>1</v>
+      </c>
+      <c r="C32" s="7">
+        <v>1</v>
+      </c>
+      <c r="D32" s="7">
+        <v>1</v>
+      </c>
+      <c r="E32" s="7">
+        <v>1</v>
+      </c>
+      <c r="F32" s="7">
+        <v>1</v>
+      </c>
+      <c r="G32" s="7">
+        <v>1</v>
+      </c>
+      <c r="H32" s="7">
+        <v>1</v>
+      </c>
+      <c r="I32" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1229,30 +1229,33 @@
       <c r="A33" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B33" s="9">
-        <v>0.73</v>
-      </c>
-      <c r="C33" s="9">
-        <v>1</v>
-      </c>
-      <c r="D33" s="9">
-        <v>1</v>
-      </c>
-      <c r="E33" s="9">
-        <v>1</v>
-      </c>
-      <c r="F33" s="9">
-        <v>0.73</v>
-      </c>
-      <c r="G33" s="9">
-        <v>1</v>
-      </c>
-      <c r="H33" s="9">
-        <v>1</v>
-      </c>
-      <c r="I33" s="9">
-        <v>1</v>
-      </c>
+      <c r="B33" s="7">
+        <v>1</v>
+      </c>
+      <c r="C33" s="7">
+        <v>1</v>
+      </c>
+      <c r="D33" s="7">
+        <v>1</v>
+      </c>
+      <c r="E33" s="7">
+        <v>1</v>
+      </c>
+      <c r="F33" s="7">
+        <v>1</v>
+      </c>
+      <c r="G33" s="7">
+        <v>1</v>
+      </c>
+      <c r="H33" s="7">
+        <v>1</v>
+      </c>
+      <c r="I33" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F34" s="7"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>

</xml_diff>

<commit_message>
Updated numbers after removing 2 molecules.
</commit_message>
<xml_diff>
--- a/ml_results.xlsx
+++ b/ml_results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timosommer/PhD/projects/others/Fukui-Indices/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A802E1B0-5C87-874D-9E60-F9F514B573D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CA3F6FA-68A0-244E-A48A-CFFF7BF3EBFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="1620" windowWidth="28800" windowHeight="17500" xr2:uid="{3179A478-D9C7-A448-B85C-D28A6D71322D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="42">
   <si>
     <t>Machine Learning results for the paper</t>
   </si>
@@ -53,21 +53,12 @@
     <t>RFC</t>
   </si>
   <si>
-    <t>2-ethyl-3-methylnaphthalene-1,4-dione</t>
-  </si>
-  <si>
     <t>2,6-bis(trifluoromethyl)pyridine</t>
   </si>
   <si>
     <t>2-(methylsulfonyl)pyrimidine</t>
   </si>
   <si>
-    <t>Pred: 0.50, True: 0.50</t>
-  </si>
-  <si>
-    <t>Pred: 0.52, True: 0.24, 0.24</t>
-  </si>
-  <si>
     <t>Pred: 0.50, True: 0.00</t>
   </si>
   <si>
@@ -101,9 +92,6 @@
     <t>uff pca 50</t>
   </si>
   <si>
-    <t>uff pca 132</t>
-  </si>
-  <si>
     <t>dft soap</t>
   </si>
   <si>
@@ -113,9 +101,6 @@
     <t>dft pca 50</t>
   </si>
   <si>
-    <t>dft pca 132</t>
-  </si>
-  <si>
     <t>Hammett</t>
   </si>
   <si>
@@ -125,21 +110,9 @@
     <t>Train accuracy (seed = 1)</t>
   </si>
   <si>
-    <t>Pred: 0.34, True: 0.33</t>
-  </si>
-  <si>
     <t>4-(pyrimidin-5-yl)benzaldehyde</t>
   </si>
   <si>
-    <t>Pred: 0.48, True: 0.01</t>
-  </si>
-  <si>
-    <t>1-(pyridin-2-yl)ethan-1-one</t>
-  </si>
-  <si>
-    <t>Pred: 0.47, True: 0.27</t>
-  </si>
-  <si>
     <t>phthalonitrile</t>
   </si>
   <si>
@@ -168,6 +141,27 @@
   </si>
   <si>
     <t>Experiment: Hammett</t>
+  </si>
+  <si>
+    <t>Pred: 0.44, True: 0.28, 0.28</t>
+  </si>
+  <si>
+    <t>Pred: 0.47, True: 0.02</t>
+  </si>
+  <si>
+    <t>uff pca 124</t>
+  </si>
+  <si>
+    <t>dft pca 124</t>
+  </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <t>The XGBC with dft soap features has 1 more wrongly predicted molecule than with uff soap features, which is 2-(trifluoromethyl)benzaldehyde  -  Pred: 0.50, True: 0.50</t>
+  </si>
+  <si>
+    <t>The LogR model on UFF SOAP features which has the same accuracy of 0.93 as the XGBC model mispredicts exactly the same two molecules.</t>
   </si>
 </sst>
 </file>
@@ -217,7 +211,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -234,11 +228,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -257,10 +288,20 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -599,8 +640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B45F95CD-8FA7-A443-A4CD-D9F038324DD6}">
   <dimension ref="A1:S81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -615,21 +656,21 @@
     <col min="11" max="11" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="F2" s="9" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="G2" s="9"/>
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
     </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -640,10 +681,10 @@
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>5</v>
@@ -652,411 +693,412 @@
         <v>6</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.93</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="G5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="3">
-        <v>0.91</v>
-      </c>
-      <c r="E5" s="4">
-        <v>1</v>
-      </c>
-      <c r="F5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D7" s="3">
-        <v>0.91</v>
+        <v>0.93</v>
       </c>
       <c r="E7" s="4">
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D9" s="3">
-        <v>0.91</v>
+        <v>0.93</v>
       </c>
       <c r="E9" s="4">
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B11">
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D11" s="3">
-        <v>0.91</v>
+        <v>0.93</v>
       </c>
       <c r="E11" s="4">
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G11" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B13">
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D13" s="3">
-        <v>0.91</v>
+        <v>0.93</v>
       </c>
       <c r="E13" s="4">
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G13" t="s">
-        <v>10</v>
-      </c>
-      <c r="H13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0.93</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.97</v>
+      </c>
+      <c r="H15" t="s">
+        <v>36</v>
+      </c>
+      <c r="I15" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="3">
-        <v>0.88</v>
-      </c>
-      <c r="E15" s="3">
-        <v>0.94</v>
-      </c>
-      <c r="F15" t="s">
-        <v>29</v>
-      </c>
-      <c r="I15" t="s">
-        <v>31</v>
-      </c>
-      <c r="J15" t="s">
-        <v>33</v>
-      </c>
-      <c r="K15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="A17" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="13"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A18" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
+      <c r="A18" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="E19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="G19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="H19" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="I19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J19" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B20" s="5">
-        <v>0.91</v>
-      </c>
-      <c r="C20" s="4">
-        <v>0.75</v>
-      </c>
-      <c r="D20" s="4">
-        <v>0.84</v>
+        <v>0.93</v>
+      </c>
+      <c r="C20" s="7">
+        <v>0.77</v>
+      </c>
+      <c r="D20" s="7">
+        <v>0.8</v>
       </c>
       <c r="E20" s="5">
-        <v>0.88</v>
+        <v>0.8</v>
       </c>
       <c r="F20" s="7">
-        <v>0.94</v>
-      </c>
-      <c r="G20" s="4">
-        <v>0.84</v>
-      </c>
-      <c r="H20" s="4">
-        <v>0.81</v>
+        <v>0.9</v>
+      </c>
+      <c r="G20" s="7">
+        <v>0.87</v>
+      </c>
+      <c r="H20" s="5">
+        <v>0.93</v>
       </c>
       <c r="I20" s="5">
-        <v>0.88</v>
+        <v>0.9</v>
+      </c>
+      <c r="J20" s="5">
+        <v>0.93</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="4">
-        <v>0.88</v>
-      </c>
-      <c r="C21" s="4">
-        <v>0.81</v>
-      </c>
-      <c r="D21" s="4">
-        <v>0.81</v>
-      </c>
-      <c r="E21" s="4">
-        <v>0.59</v>
-      </c>
-      <c r="F21" s="4">
-        <v>0.94</v>
-      </c>
-      <c r="G21" s="4">
-        <v>0.81</v>
-      </c>
-      <c r="H21" s="4">
-        <v>0.81</v>
-      </c>
-      <c r="I21" s="4">
-        <v>0.75</v>
+      <c r="B21" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="C21" s="5">
+        <v>0.83</v>
+      </c>
+      <c r="D21" s="7">
+        <v>0.83</v>
+      </c>
+      <c r="E21" s="7">
+        <v>0.63</v>
+      </c>
+      <c r="F21" s="7">
+        <v>0.93</v>
+      </c>
+      <c r="G21" s="7">
+        <v>0.87</v>
+      </c>
+      <c r="H21" s="7">
+        <v>0.87</v>
+      </c>
+      <c r="I21" s="7">
+        <v>0.73</v>
+      </c>
+      <c r="J21" s="7">
+        <v>0.87</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" s="4">
-        <v>0.88</v>
+        <v>9</v>
+      </c>
+      <c r="B22" s="5">
+        <v>0.93</v>
       </c>
       <c r="C22" s="5">
-        <v>0.84</v>
+        <v>0.83</v>
       </c>
       <c r="D22" s="5">
-        <v>0.94</v>
-      </c>
-      <c r="E22" s="4">
-        <v>0.09</v>
+        <v>0.9</v>
+      </c>
+      <c r="E22" s="7">
+        <v>0.13</v>
       </c>
       <c r="F22" s="5">
         <v>0.97</v>
       </c>
       <c r="G22" s="5">
-        <v>0.91</v>
-      </c>
-      <c r="H22" s="5">
-        <v>0.91</v>
-      </c>
-      <c r="I22" s="4">
-        <v>0.09</v>
+        <v>0.9</v>
+      </c>
+      <c r="H22" s="7">
+        <v>0.87</v>
+      </c>
+      <c r="I22" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="J22" s="7">
+        <v>0.47</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="4">
-        <v>0.78</v>
-      </c>
-      <c r="C23" s="4">
-        <v>0.81</v>
-      </c>
-      <c r="D23" s="7">
-        <v>0.91</v>
-      </c>
-      <c r="E23" s="4">
+        <v>10</v>
+      </c>
+      <c r="B23" s="7">
+        <v>0.83</v>
+      </c>
+      <c r="C23" s="5">
+        <v>0.83</v>
+      </c>
+      <c r="D23" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="E23" s="7">
         <v>0.03</v>
       </c>
-      <c r="F23" s="4">
-        <v>0.84</v>
+      <c r="F23" s="7">
+        <v>0.87</v>
       </c>
       <c r="G23" s="7">
-        <v>0.88</v>
-      </c>
-      <c r="H23" s="4">
-        <v>0.88</v>
-      </c>
-      <c r="I23" s="4">
-        <v>0.06</v>
+        <v>0.83</v>
+      </c>
+      <c r="H23" s="7">
+        <v>0.87</v>
+      </c>
+      <c r="I23" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="J23" s="7">
+        <v>0.7</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" s="4">
-        <v>0.06</v>
-      </c>
-      <c r="C24" s="4">
-        <v>0.75</v>
-      </c>
-      <c r="D24" s="4">
-        <v>0.72</v>
-      </c>
-      <c r="E24" s="4">
+        <v>11</v>
+      </c>
+      <c r="B24" s="7">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C24" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="D24" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="E24" s="7">
         <v>0</v>
       </c>
-      <c r="F24" s="4">
-        <v>0.06</v>
-      </c>
-      <c r="G24" s="4">
-        <v>0.81</v>
-      </c>
-      <c r="H24" s="4">
-        <v>0.72</v>
-      </c>
-      <c r="I24" s="4">
+      <c r="F24" s="7">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G24" s="7">
+        <v>0.73</v>
+      </c>
+      <c r="H24" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="I24" s="7">
         <v>0</v>
+      </c>
+      <c r="J24" s="7">
+        <v>0.63</v>
       </c>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
@@ -1068,50 +1110,54 @@
       <c r="S24" s="3"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A27" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
+      <c r="A27" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="E28" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F28" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="G28" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="H28" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="I28" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J28" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B29" s="7">
         <v>1</v>
@@ -1136,6 +1182,9 @@
       </c>
       <c r="I29" s="7">
         <v>1</v>
+      </c>
+      <c r="J29" s="7">
+        <v>0.97</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.2">
@@ -1166,10 +1215,13 @@
       <c r="I30" s="7">
         <v>1</v>
       </c>
+      <c r="J30" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B31" s="7">
         <v>1</v>
@@ -1195,10 +1247,13 @@
       <c r="I31" s="7">
         <v>1</v>
       </c>
+      <c r="J31" s="7">
+        <v>0.48</v>
+      </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B32" s="7">
         <v>1</v>
@@ -1224,10 +1279,13 @@
       <c r="I32" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J32" s="7">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B33" s="7">
         <v>1</v>
@@ -1253,14 +1311,32 @@
       <c r="I33" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J33" s="7">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="F34" s="7"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
@@ -1282,10 +1358,11 @@
       <c r="A81" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A18:I18"/>
-    <mergeCell ref="A27:I27"/>
+  <mergeCells count="4">
     <mergeCell ref="F2:J2"/>
+    <mergeCell ref="A18:J18"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A17:J17"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>